<commit_message>
do one math question.
</commit_message>
<xml_diff>
--- a/exer/move.xlsx
+++ b/exer/move.xlsx
@@ -1,49 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minghao/PycharmProjects/LearningPython/exer/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74C71B5-6D00-A140-99D0-5B88E28CEFF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16440" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <name val="等线"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="等线"/>
-      <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="006187b4"/>
-        <bgColor rgb="006187b4"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -56,18 +48,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -333,209 +332,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="F5:V21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD14" sqref="AD14"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="5.625" defaultRowHeight="20.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="2" width="5.625"/>
-    <col customWidth="1" max="16384" min="3" style="2" width="5.625"/>
+    <col min="1" max="7" width="5.6640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="5.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="20.1" r="4" s="2"/>
-    <row r="5">
-      <c r="N5" s="3" t="n"/>
-    </row>
-    <row r="6">
-      <c r="M6" s="3" t="n"/>
-      <c r="N6" s="3" t="n"/>
-      <c r="O6" s="3" t="n"/>
-    </row>
-    <row r="7">
-      <c r="L7" s="3" t="n"/>
-      <c r="M7" s="3" t="n"/>
-      <c r="N7" s="3" t="n"/>
-      <c r="O7" s="3" t="n"/>
-      <c r="P7" s="3" t="n"/>
-    </row>
-    <row r="8">
-      <c r="K8" s="3" t="n"/>
-      <c r="L8" s="3" t="n"/>
-      <c r="M8" s="3" t="n"/>
-      <c r="N8" s="3" t="n"/>
-      <c r="O8" s="3" t="n"/>
-      <c r="P8" s="3" t="n"/>
-      <c r="Q8" s="3" t="n"/>
-    </row>
-    <row r="9">
-      <c r="J9" s="3" t="n"/>
-      <c r="K9" s="3" t="n"/>
-      <c r="L9" s="3" t="n"/>
-      <c r="M9" s="3" t="n"/>
-      <c r="N9" s="3" t="n"/>
-      <c r="O9" s="3" t="n"/>
-      <c r="P9" s="3" t="n"/>
-      <c r="Q9" s="3" t="n"/>
-      <c r="R9" s="3" t="n"/>
-    </row>
-    <row r="10">
-      <c r="I10" s="3" t="n"/>
-      <c r="J10" s="3" t="n"/>
-      <c r="K10" s="3" t="n"/>
-      <c r="L10" s="3" t="n"/>
-      <c r="M10" s="3" t="n"/>
-      <c r="N10" s="3" t="n"/>
-      <c r="O10" s="3" t="n"/>
-      <c r="P10" s="3" t="n"/>
-      <c r="Q10" s="3" t="n"/>
-      <c r="R10" s="3" t="n"/>
-      <c r="S10" s="3" t="n"/>
-    </row>
-    <row r="11">
-      <c r="H11" s="3" t="n"/>
-      <c r="I11" s="3" t="n"/>
-      <c r="J11" s="3" t="n"/>
-      <c r="K11" s="3" t="n"/>
-      <c r="L11" s="3" t="n"/>
-      <c r="M11" s="3" t="n"/>
-      <c r="N11" s="3" t="n"/>
-      <c r="O11" s="3" t="n"/>
-      <c r="P11" s="3" t="n"/>
-      <c r="Q11" s="3" t="n"/>
-      <c r="R11" s="3" t="n"/>
-      <c r="S11" s="3" t="n"/>
-      <c r="T11" s="3" t="n"/>
-    </row>
-    <row r="12">
-      <c r="G12" s="3" t="n"/>
-      <c r="H12" s="3" t="n"/>
-      <c r="I12" s="3" t="n"/>
-      <c r="J12" s="3" t="n"/>
-      <c r="K12" s="3" t="n"/>
-      <c r="L12" s="3" t="n"/>
-      <c r="M12" s="3" t="n"/>
-      <c r="N12" s="3" t="n"/>
-      <c r="O12" s="3" t="n"/>
-      <c r="P12" s="3" t="n"/>
-      <c r="Q12" s="3" t="n"/>
-      <c r="R12" s="3" t="n"/>
-      <c r="S12" s="3" t="n"/>
-      <c r="T12" s="3" t="n"/>
-      <c r="U12" s="3" t="n"/>
-    </row>
-    <row r="13">
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
-      <c r="H13" s="3" t="n"/>
-      <c r="I13" s="3" t="n"/>
-      <c r="J13" s="3" t="n"/>
-      <c r="K13" s="3" t="n"/>
-      <c r="L13" s="3" t="n"/>
-      <c r="M13" s="3" t="n"/>
-      <c r="N13" s="3" t="n"/>
-      <c r="O13" s="3" t="n"/>
-      <c r="P13" s="3" t="n"/>
-      <c r="Q13" s="3" t="n"/>
-      <c r="R13" s="3" t="n"/>
-      <c r="S13" s="3" t="n"/>
-      <c r="T13" s="3" t="n"/>
-      <c r="U13" s="3" t="n"/>
-      <c r="V13" s="3" t="n"/>
-    </row>
-    <row r="14">
-      <c r="G14" s="3" t="n"/>
-      <c r="H14" s="3" t="n"/>
-      <c r="I14" s="3" t="n"/>
-      <c r="J14" s="3" t="n"/>
-      <c r="K14" s="3" t="n"/>
-      <c r="L14" s="3" t="n"/>
-      <c r="M14" s="3" t="n"/>
-      <c r="N14" s="3" t="n"/>
-      <c r="O14" s="3" t="n"/>
-      <c r="P14" s="3" t="n"/>
-      <c r="Q14" s="3" t="n"/>
-      <c r="R14" s="3" t="n"/>
-      <c r="S14" s="3" t="n"/>
-      <c r="T14" s="3" t="n"/>
-      <c r="U14" s="3" t="n"/>
-    </row>
-    <row r="15">
-      <c r="H15" s="3" t="n"/>
-      <c r="I15" s="3" t="n"/>
-      <c r="J15" s="3" t="n"/>
-      <c r="K15" s="3" t="n"/>
-      <c r="L15" s="3" t="n"/>
-      <c r="M15" s="3" t="n"/>
-      <c r="N15" s="3" t="n"/>
-      <c r="O15" s="3" t="n"/>
-      <c r="P15" s="3" t="n"/>
-      <c r="Q15" s="3" t="n"/>
-      <c r="R15" s="3" t="n"/>
-      <c r="S15" s="3" t="n"/>
-      <c r="T15" s="3" t="n"/>
-    </row>
-    <row r="16">
-      <c r="I16" s="3" t="n"/>
-      <c r="J16" s="3" t="n"/>
-      <c r="K16" s="3" t="n"/>
-      <c r="L16" s="3" t="n"/>
-      <c r="M16" s="3" t="n"/>
-      <c r="N16" s="3" t="n"/>
-      <c r="O16" s="3" t="n"/>
-      <c r="P16" s="3" t="n"/>
-      <c r="Q16" s="3" t="n"/>
-      <c r="R16" s="3" t="n"/>
-      <c r="S16" s="3" t="n"/>
-    </row>
-    <row r="17">
-      <c r="J17" s="3" t="n"/>
-      <c r="K17" s="3" t="n"/>
-      <c r="L17" s="3" t="n"/>
-      <c r="M17" s="3" t="n"/>
-      <c r="N17" s="3" t="n"/>
-      <c r="O17" s="3" t="n"/>
-      <c r="P17" s="3" t="n"/>
-      <c r="Q17" s="3" t="n"/>
-      <c r="R17" s="3" t="n"/>
-    </row>
-    <row r="18">
-      <c r="K18" s="3" t="n"/>
-      <c r="L18" s="3" t="n"/>
-      <c r="M18" s="3" t="n"/>
-      <c r="N18" s="3" t="n"/>
-      <c r="O18" s="3" t="n"/>
-      <c r="P18" s="3" t="n"/>
-      <c r="Q18" s="3" t="n"/>
-    </row>
-    <row r="19">
-      <c r="L19" s="3" t="n"/>
-      <c r="M19" s="3" t="n"/>
-      <c r="N19" s="3" t="n"/>
-      <c r="O19" s="3" t="n"/>
-      <c r="P19" s="3" t="n"/>
-    </row>
-    <row r="20">
-      <c r="M20" s="3" t="n"/>
-      <c r="N20" s="3" t="n"/>
-      <c r="O20" s="3" t="n"/>
-    </row>
-    <row r="21">
-      <c r="N21" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="20.1" r="22" s="2"/>
-    <row customHeight="1" ht="20.1" r="23" s="2"/>
-    <row customHeight="1" ht="20.1" r="24" s="2"/>
-    <row customHeight="1" ht="20.1" r="25" s="2"/>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>